<commit_message>
test nomina con delete
</commit_message>
<xml_diff>
--- a/Payroll/Nomina.xlsx
+++ b/Payroll/Nomina.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Nomina" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculo_nomina" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>totalRevenue</t>
   </si>
@@ -77,15 +78,6 @@
     <t>month</t>
   </si>
   <si>
-    <t>Nomina Enero 202</t>
-  </si>
-  <si>
-    <t>Nomina Enero 203</t>
-  </si>
-  <si>
-    <t>Nomina Enero 204</t>
-  </si>
-  <si>
     <t>propertyEmployees</t>
   </si>
   <si>
@@ -93,13 +85,61 @@
   </si>
   <si>
     <t>fullName</t>
+  </si>
+  <si>
+    <t>kjhdasja</t>
+  </si>
+  <si>
+    <t>identification</t>
+  </si>
+  <si>
+    <t>usersCode</t>
+  </si>
+  <si>
+    <t>contractCode</t>
+  </si>
+  <si>
+    <t>fklaejdoiajraw</t>
+  </si>
+  <si>
+    <t>employeesData</t>
+  </si>
+  <si>
+    <t>Nombretabla</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>stringResponseCreate</t>
+  </si>
+  <si>
+    <t>is an invalid start of a value. Path:</t>
+  </si>
+  <si>
+    <t>PayrollPeriodID</t>
+  </si>
+  <si>
+    <t>Nomina Enero 2021</t>
+  </si>
+  <si>
+    <t>payrollPeriodIdTest</t>
+  </si>
+  <si>
+    <t>statusGetPayroll</t>
+  </si>
+  <si>
+    <t>statusDelete</t>
+  </si>
+  <si>
+    <t>statusCreate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,13 +161,43 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,16 +209,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -448,61 +524,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="33" customWidth="1"/>
-    <col min="12" max="12" width="29.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="33" customWidth="1"/>
+    <col min="14" max="17" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="O1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -513,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>2021</v>
@@ -521,26 +615,42 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
+      <c r="O2">
+        <v>200</v>
+      </c>
+      <c r="Q2">
+        <v>200</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(AND(P2="",H2=400),"The value 'null' is not valid.",IF(ISNUMBER(P2),"Bad Request",IF(OR(P2="",H2=200),IF(H2=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P2&amp;"' is not valid.")))</f>
+        <v>Payroll Deleted</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -551,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>2021</v>
@@ -559,26 +669,42 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>13</v>
       </c>
+      <c r="O3">
+        <v>200</v>
+      </c>
+      <c r="Q3">
+        <v>200</v>
+      </c>
+      <c r="R3" t="str">
+        <f>IF(AND(P3="",H3=400),"The value 'null' is not valid.",IF(ISNUMBER(P3),"Bad Request",IF(OR(P3="",H3=200),IF(H3=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P3&amp;"' is not valid.")))</f>
+        <v>Payroll Deleted</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -589,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>2021</v>
@@ -597,32 +723,200 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>13</v>
+      </c>
+      <c r="O4">
+        <v>200</v>
+      </c>
+      <c r="Q4">
+        <v>200</v>
+      </c>
+      <c r="R4" t="str">
+        <f>IF(AND(P4="",H4=400),"The value 'null' is not valid.",IF(ISNUMBER(P4),"Bad Request",IF(OR(P4="",H4=200),IF(H4=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P4&amp;"' is not valid.")))</f>
+        <v>Payroll Deleted</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
+        <v>400</v>
+      </c>
+      <c r="O5">
+        <v>400</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>400</v>
+      </c>
+      <c r="R5" t="str">
+        <f>IF(AND(P5="",H5=400),"The value 'null' is not valid.",IF(ISNUMBER(P5),"Bad Request",IF(OR(P5="",H5=200),IF(H5=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P5&amp;"' is not valid.")))</f>
+        <v>Bad Request</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6">
+        <v>400</v>
+      </c>
+      <c r="O6">
+        <v>400</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <v>400</v>
+      </c>
+      <c r="R6" t="str">
+        <f>IF(AND(P6="",H6=400),"The value 'null' is not valid.",IF(ISNUMBER(P6),"Bad Request",IF(OR(P6="",H6=200),IF(H6=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P6&amp;"' is not valid.")))</f>
+        <v>The value 'kjhdasja' is not valid.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <v>400</v>
+      </c>
+      <c r="O7">
+        <v>404</v>
+      </c>
+      <c r="Q7">
+        <v>404</v>
+      </c>
+      <c r="R7" t="str">
+        <f>IF(AND(P7="",H7=400),"The value 'null' is not valid.",IF(ISNUMBER(P7),"Bad Request",IF(OR(P7="",H7=200),IF(H7=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P7&amp;"' is not valid.")))</f>
+        <v>The value 'null' is not valid.</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2222</v>
+      </c>
+      <c r="H8">
+        <v>401</v>
+      </c>
+      <c r="O8">
+        <v>404</v>
+      </c>
+      <c r="Q8">
+        <v>404</v>
+      </c>
+      <c r="R8" t="str">
+        <f>IF(AND(P8="",H8=400),"The value 'null' is not valid.",IF(ISNUMBER(P8),"Bad Request",IF(OR(P8="",H8=200),IF(H8=401,"Unauthorized","Payroll Deleted"),"The value '"&amp;P8&amp;"' is not valid.")))</f>
+        <v>Unauthorized</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>456465</v>
+      </c>
+      <c r="C2">
+        <v>113022222</v>
+      </c>
+      <c r="D2">
+        <v>63632</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nuevo archivo de nomina2
</commit_message>
<xml_diff>
--- a/Payroll/Nomina.xlsx
+++ b/Payroll/Nomina.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2232"/>
   </bookViews>
   <sheets>
     <sheet name="Nomina" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>totalRevenue</t>
   </si>
@@ -114,9 +114,6 @@
     <t>stringResponseCreate</t>
   </si>
   <si>
-    <t>is an invalid start of a value. Path:</t>
-  </si>
-  <si>
     <t>PayrollPeriodID</t>
   </si>
   <si>
@@ -139,6 +136,15 @@
   </si>
   <si>
     <t>http://23.101.145.208:50000</t>
+  </si>
+  <si>
+    <t>is an invalid start of a value. Path: $.periodType</t>
+  </si>
+  <si>
+    <t>is an invalid start of a value. Path: $.year</t>
+  </si>
+  <si>
+    <t>is an invalid start of a value. Path: $.month</t>
   </si>
 </sst>
 </file>
@@ -539,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +561,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
@@ -579,7 +585,7 @@
         <v>28</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -600,13 +606,13 @@
         <v>2</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>27</v>
@@ -614,7 +620,7 @@
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -626,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>2021</v>
@@ -635,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2">
         <v>200</v>
@@ -671,7 +677,7 @@
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -683,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>2021</v>
@@ -692,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>200</v>
@@ -728,7 +734,7 @@
     </row>
     <row r="4" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -740,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>2021</v>
@@ -749,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>200</v>
@@ -785,7 +791,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -794,7 +800,7 @@
         <v>1111</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I5">
         <v>400</v>
@@ -815,7 +821,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -823,8 +829,11 @@
       <c r="C6">
         <v>1111</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I6">
         <v>400</v>
@@ -845,7 +854,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -853,17 +862,23 @@
       <c r="C7">
         <v>1111</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2021</v>
+      </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I7">
         <v>400</v>
       </c>
       <c r="P7">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="R7">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="0"/>
@@ -872,7 +887,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -884,10 +899,10 @@
         <v>401</v>
       </c>
       <c r="P8">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="R8">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
@@ -916,7 +931,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>